<commit_message>
Excel read in categoryPage.java done
</commit_message>
<xml_diff>
--- a/GroceryApplication/src/main/resources/Excel/GroceryApplicationData.xlsx
+++ b/GroceryApplication/src/main/resources/Excel/GroceryApplicationData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eclipse_Workspace\GroceryApplication\src\main\resources\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AISWARYA\git\Grocery-Application\GroceryApplication\src\main\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61FAE83F-2A4F-47BD-987B-6C835FBC4126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44E1239-E2D5-4667-831A-6EA9708BA163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -397,12 +397,12 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="25.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -417,7 +417,7 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>